<commit_message>
Commit connected all the program
</commit_message>
<xml_diff>
--- a/dsalgoProject/src/test/resources/ExcelData/TestData.xlsx
+++ b/dsalgoProject/src/test/resources/ExcelData/TestData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{DB09F419-BFB7-4B4F-9D3A-83B2BFDA2C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\senth\git\dsalgo_Demo\dsalgoProject\src\test\resources\ExcelData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C1C61A-DEFC-4DCC-ABE7-290BE44D97B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:P4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>print('Hello')</t>
   </si>
@@ -56,6 +60,9 @@
   </si>
   <si>
     <t>print("Hello")</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -378,7 +385,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -457,10 +464,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC84688-0A32-43F9-A143-ADB30766B200}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,6 +485,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>